<commit_message>
3.1.6: Separate BodyTelegram from PlainRquestTelegram.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestGeneratorKtTelegramStructure.xlsx
+++ b/meta/program/BlancoRestGeneratorKtTelegramStructure.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/vscode/blanco/blancoRestGeneratorKt/meta/program/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorKt/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2FF3FF-9D76-EC43-ADF8-41C38F842C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5C6E58-C9AA-5F49-8047-4690941AECD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2660" yWindow="11300" windowWidth="24320" windowHeight="17500" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="104">
   <si>
     <t>バリューオブジェクト定義書</t>
   </si>
@@ -578,6 +578,33 @@
     </rPh>
     <rPh sb="16" eb="18">
       <t xml:space="preserve">ホゾｎ </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>bodyTelegram</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>blanco.restgeneratorkt.valueobject.BlancoRestGeneratorKtTelegramStructure</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>PathとQueryで指定されるプロパティを除いた、bodyにJSONとして乗せられるプロパティだけを集約した電文です。</t>
+    <rPh sb="11" eb="13">
+      <t xml:space="preserve">シテイ </t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t xml:space="preserve">ノゾイタ </t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t xml:space="preserve">ノセラレル </t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t xml:space="preserve">シュウヤク </t>
+    </rPh>
+    <rPh sb="55" eb="57">
+      <t xml:space="preserve">デンブｎ </t>
     </rPh>
     <phoneticPr fontId="4"/>
   </si>
@@ -1684,10 +1711,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57:F57"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1973,7 +2000,7 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="29">
-        <f t="shared" ref="A29:A56" si="0">A28+1</f>
+        <f t="shared" ref="A29:A57" si="0">A28+1</f>
         <v>3</v>
       </c>
       <c r="B29" s="30" t="s">
@@ -2493,34 +2520,52 @@
       <c r="F56" s="54"/>
       <c r="G56"/>
     </row>
-    <row r="57" spans="1:7" s="45" customFormat="1" ht="15" customHeight="1">
-      <c r="A57" s="29"/>
-      <c r="B57" s="43"/>
-      <c r="C57" s="44"/>
-      <c r="D57" s="44"/>
-      <c r="E57" s="53"/>
+    <row r="57" spans="1:7" s="45" customFormat="1" ht="45">
+      <c r="A57" s="29">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B57" s="48" t="s">
+        <v>101</v>
+      </c>
+      <c r="C57" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="D57" s="49"/>
+      <c r="E57" s="53" t="s">
+        <v>103</v>
+      </c>
       <c r="F57" s="54"/>
       <c r="G57"/>
     </row>
-    <row r="58" spans="1:7" s="45" customFormat="1">
-      <c r="A58" s="52"/>
-      <c r="B58" s="48"/>
+    <row r="58" spans="1:7" s="45" customFormat="1" ht="15" customHeight="1">
+      <c r="A58" s="29"/>
+      <c r="B58" s="43"/>
       <c r="C58" s="44"/>
-      <c r="D58" s="49"/>
+      <c r="D58" s="44"/>
       <c r="E58" s="53"/>
       <c r="F58" s="54"/>
       <c r="G58"/>
     </row>
-    <row r="59" spans="1:7">
-      <c r="A59" s="22"/>
-      <c r="B59" s="34"/>
-      <c r="C59" s="23"/>
-      <c r="D59" s="23"/>
-      <c r="E59" s="23"/>
-      <c r="F59" s="35"/>
+    <row r="59" spans="1:7" s="45" customFormat="1">
+      <c r="A59" s="52"/>
+      <c r="B59" s="48"/>
+      <c r="C59" s="44"/>
+      <c r="D59" s="49"/>
+      <c r="E59" s="53"/>
+      <c r="F59" s="54"/>
+      <c r="G59"/>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" s="22"/>
+      <c r="B60" s="34"/>
+      <c r="C60" s="23"/>
+      <c r="D60" s="23"/>
+      <c r="E60" s="23"/>
+      <c r="F60" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
+  <mergeCells count="35">
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:B20"/>
@@ -2547,18 +2592,19 @@
     <mergeCell ref="E51:F51"/>
     <mergeCell ref="E47:F47"/>
     <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="E59:F59"/>
     <mergeCell ref="E49:F49"/>
     <mergeCell ref="E52:F52"/>
     <mergeCell ref="E53:F53"/>
     <mergeCell ref="E54:F54"/>
-    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="E58:F58"/>
     <mergeCell ref="E55:F55"/>
     <mergeCell ref="E56:F56"/>
+    <mergeCell ref="E57:F57"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations disablePrompts="1" count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D75" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D76" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Adapt primitive array for response.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestGeneratorKtTelegramStructure.xlsx
+++ b/meta/program/BlancoRestGeneratorKtTelegramStructure.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorKt/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52BB36E9-7477-CC4D-8A51-1A1779303B44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF4BD3D-EE93-0A4C-BF66-5FB73E6DAD4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2660" yWindow="3500" windowWidth="24320" windowHeight="17500" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="113">
   <si>
     <t>バリューオブジェクト定義書</t>
   </si>
@@ -659,6 +659,20 @@
       <t xml:space="preserve">ハイレツ </t>
     </rPh>
     <rPh sb="12" eb="13">
+      <t xml:space="preserve">ノル </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>primitivePayload</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>ペイロードにprimitive (非JSON）が載る</t>
+    <rPh sb="17" eb="18">
+      <t xml:space="preserve">ヒ </t>
+    </rPh>
+    <rPh sb="24" eb="25">
       <t xml:space="preserve">ノル </t>
     </rPh>
     <phoneticPr fontId="4"/>
@@ -1264,6 +1278,27 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1284,27 +1319,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1697,7 +1711,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1741,7 +1755,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1766,10 +1780,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61:F61"/>
+      <selection activeCell="E42" sqref="E42:F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1942,23 +1956,23 @@
       <c r="F18"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="55" t="s">
+      <c r="A19" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="56" t="s">
+      <c r="B19" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="57"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="58"/>
+      <c r="C19" s="64"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="65"/>
       <c r="F19"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="55"/>
-      <c r="B20" s="56"/>
-      <c r="C20" s="57"/>
-      <c r="D20" s="57"/>
-      <c r="E20" s="58"/>
+      <c r="A20" s="62"/>
+      <c r="B20" s="63"/>
+      <c r="C20" s="64"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="65"/>
       <c r="F20"/>
     </row>
     <row r="21" spans="1:6">
@@ -1995,29 +2009,29 @@
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:6" ht="13.5" customHeight="1">
-      <c r="A25" s="55" t="s">
+      <c r="A25" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="55" t="s">
+      <c r="B25" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="59" t="s">
+      <c r="C25" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="D25" s="59" t="s">
+      <c r="D25" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="59" t="s">
+      <c r="E25" s="66" t="s">
         <v>7</v>
       </c>
       <c r="F25" s="26"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="55"/>
-      <c r="B26" s="55"/>
-      <c r="C26" s="59"/>
-      <c r="D26" s="59"/>
-      <c r="E26" s="59"/>
+      <c r="A26" s="62"/>
+      <c r="B26" s="62"/>
+      <c r="C26" s="66"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="66"/>
       <c r="F26" s="27"/>
     </row>
     <row r="27" spans="1:6">
@@ -2031,10 +2045,10 @@
         <v>24</v>
       </c>
       <c r="D27" s="19"/>
-      <c r="E27" s="53" t="s">
+      <c r="E27" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="F27" s="54"/>
+      <c r="F27" s="61"/>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="29">
@@ -2055,7 +2069,7 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="29">
-        <f t="shared" ref="A29:A60" si="0">A28+1</f>
+        <f t="shared" ref="A29:A61" si="0">A28+1</f>
         <v>3</v>
       </c>
       <c r="B29" s="30" t="s">
@@ -2169,10 +2183,10 @@
       <c r="D35" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="E35" s="62" t="s">
+      <c r="E35" s="55" t="s">
         <v>49</v>
       </c>
-      <c r="F35" s="63"/>
+      <c r="F35" s="56"/>
       <c r="G35"/>
     </row>
     <row r="36" spans="1:7" s="45" customFormat="1" ht="15">
@@ -2189,10 +2203,10 @@
       <c r="D36" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="E36" s="60" t="s">
+      <c r="E36" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="F36" s="61"/>
+      <c r="F36" s="54"/>
       <c r="G36"/>
     </row>
     <row r="37" spans="1:7" s="45" customFormat="1" ht="15">
@@ -2207,10 +2221,10 @@
         <v>24</v>
       </c>
       <c r="D37" s="44"/>
-      <c r="E37" s="60" t="s">
+      <c r="E37" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="F37" s="61"/>
+      <c r="F37" s="54"/>
       <c r="G37"/>
     </row>
     <row r="38" spans="1:7" s="45" customFormat="1" ht="45" customHeight="1">
@@ -2227,10 +2241,10 @@
       <c r="D38" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="E38" s="60" t="s">
+      <c r="E38" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="F38" s="66"/>
+      <c r="F38" s="59"/>
       <c r="G38"/>
     </row>
     <row r="39" spans="1:7" s="45" customFormat="1" ht="45">
@@ -2247,10 +2261,10 @@
       <c r="D39" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="E39" s="60" t="s">
+      <c r="E39" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="F39" s="61"/>
+      <c r="F39" s="54"/>
       <c r="G39"/>
     </row>
     <row r="40" spans="1:7" s="45" customFormat="1" ht="45">
@@ -2267,10 +2281,10 @@
       <c r="D40" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="E40" s="64" t="s">
+      <c r="E40" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="F40" s="65"/>
+      <c r="F40" s="58"/>
       <c r="G40"/>
     </row>
     <row r="41" spans="1:7">
@@ -2306,10 +2320,10 @@
       <c r="D42" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="E42" s="60" t="s">
+      <c r="E42" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="F42" s="61"/>
+      <c r="F42" s="54"/>
     </row>
     <row r="43" spans="1:7" ht="15">
       <c r="A43" s="29">
@@ -2325,10 +2339,10 @@
       <c r="D43" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="E43" s="60" t="s">
+      <c r="E43" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="F43" s="61"/>
+      <c r="F43" s="54"/>
     </row>
     <row r="44" spans="1:7" ht="15">
       <c r="A44" s="29">
@@ -2344,10 +2358,10 @@
       <c r="D44" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="E44" s="60" t="s">
+      <c r="E44" s="53" t="s">
         <v>73</v>
       </c>
-      <c r="F44" s="61"/>
+      <c r="F44" s="54"/>
     </row>
     <row r="45" spans="1:7" s="45" customFormat="1" ht="15">
       <c r="A45" s="29">
@@ -2363,10 +2377,10 @@
       <c r="D45" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="E45" s="60" t="s">
+      <c r="E45" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="F45" s="61"/>
+      <c r="F45" s="54"/>
       <c r="G45"/>
     </row>
     <row r="46" spans="1:7" s="45" customFormat="1">
@@ -2383,10 +2397,10 @@
       <c r="D46" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="E46" s="60" t="s">
+      <c r="E46" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="F46" s="61"/>
+      <c r="F46" s="54"/>
       <c r="G46"/>
     </row>
     <row r="47" spans="1:7" s="45" customFormat="1" ht="15">
@@ -2401,10 +2415,10 @@
         <v>34</v>
       </c>
       <c r="D47" s="49"/>
-      <c r="E47" s="60" t="s">
+      <c r="E47" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="F47" s="61"/>
+      <c r="F47" s="54"/>
       <c r="G47"/>
     </row>
     <row r="48" spans="1:7" s="45" customFormat="1" ht="15">
@@ -2419,10 +2433,10 @@
         <v>34</v>
       </c>
       <c r="D48" s="49"/>
-      <c r="E48" s="60" t="s">
+      <c r="E48" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="F48" s="61"/>
+      <c r="F48" s="54"/>
       <c r="G48"/>
     </row>
     <row r="49" spans="1:7" s="45" customFormat="1" ht="15">
@@ -2437,10 +2451,10 @@
         <v>34</v>
       </c>
       <c r="D49" s="49"/>
-      <c r="E49" s="60" t="s">
+      <c r="E49" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="F49" s="61"/>
+      <c r="F49" s="54"/>
       <c r="G49"/>
     </row>
     <row r="50" spans="1:7" s="45" customFormat="1" ht="15" customHeight="1">
@@ -2457,10 +2471,10 @@
       <c r="D50" s="44" t="b">
         <v>0</v>
       </c>
-      <c r="E50" s="60" t="s">
+      <c r="E50" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="F50" s="61"/>
+      <c r="F50" s="54"/>
       <c r="G50"/>
     </row>
     <row r="51" spans="1:7" s="45" customFormat="1" ht="15" customHeight="1">
@@ -2475,10 +2489,10 @@
         <v>34</v>
       </c>
       <c r="D51" s="44"/>
-      <c r="E51" s="60" t="s">
+      <c r="E51" s="53" t="s">
         <v>89</v>
       </c>
-      <c r="F51" s="61"/>
+      <c r="F51" s="54"/>
       <c r="G51"/>
     </row>
     <row r="52" spans="1:7" s="45" customFormat="1" ht="15" customHeight="1">
@@ -2493,10 +2507,10 @@
         <v>34</v>
       </c>
       <c r="D52" s="44"/>
-      <c r="E52" s="60" t="s">
+      <c r="E52" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="F52" s="61"/>
+      <c r="F52" s="54"/>
       <c r="G52"/>
     </row>
     <row r="53" spans="1:7" s="45" customFormat="1" ht="15" customHeight="1">
@@ -2511,10 +2525,10 @@
         <v>34</v>
       </c>
       <c r="D53" s="44"/>
-      <c r="E53" s="60" t="s">
+      <c r="E53" s="53" t="s">
         <v>93</v>
       </c>
-      <c r="F53" s="61"/>
+      <c r="F53" s="54"/>
       <c r="G53"/>
     </row>
     <row r="54" spans="1:7" s="45" customFormat="1" ht="15" customHeight="1">
@@ -2531,10 +2545,10 @@
       <c r="D54" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="60" t="s">
+      <c r="E54" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="F54" s="61"/>
+      <c r="F54" s="54"/>
       <c r="G54"/>
     </row>
     <row r="55" spans="1:7" s="45" customFormat="1" ht="15" customHeight="1">
@@ -2551,10 +2565,10 @@
       <c r="D55" s="44" t="b">
         <v>0</v>
       </c>
-      <c r="E55" s="60" t="s">
+      <c r="E55" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="F55" s="61"/>
+      <c r="F55" s="54"/>
       <c r="G55"/>
     </row>
     <row r="56" spans="1:7" s="45" customFormat="1" ht="15">
@@ -2569,10 +2583,10 @@
         <v>34</v>
       </c>
       <c r="D56" s="49"/>
-      <c r="E56" s="60" t="s">
+      <c r="E56" s="53" t="s">
         <v>100</v>
       </c>
-      <c r="F56" s="61"/>
+      <c r="F56" s="54"/>
       <c r="G56"/>
     </row>
     <row r="57" spans="1:7" s="45" customFormat="1" ht="45">
@@ -2587,10 +2601,10 @@
         <v>102</v>
       </c>
       <c r="D57" s="49"/>
-      <c r="E57" s="60" t="s">
+      <c r="E57" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="F57" s="61"/>
+      <c r="F57" s="54"/>
       <c r="G57"/>
     </row>
     <row r="58" spans="1:7" s="45" customFormat="1" ht="15">
@@ -2607,10 +2621,10 @@
       <c r="D58" s="49" t="s">
         <v>105</v>
       </c>
-      <c r="E58" s="60" t="s">
+      <c r="E58" s="53" t="s">
         <v>106</v>
       </c>
-      <c r="F58" s="61"/>
+      <c r="F58" s="54"/>
       <c r="G58"/>
     </row>
     <row r="59" spans="1:7" s="45" customFormat="1" ht="15">
@@ -2627,10 +2641,10 @@
       <c r="D59" s="49" t="b">
         <v>0</v>
       </c>
-      <c r="E59" s="60" t="s">
+      <c r="E59" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="F59" s="61"/>
+      <c r="F59" s="54"/>
       <c r="G59"/>
     </row>
     <row r="60" spans="1:7" s="45" customFormat="1" ht="15">
@@ -2647,67 +2661,61 @@
       <c r="D60" s="49" t="b">
         <v>0</v>
       </c>
-      <c r="E60" s="60" t="s">
+      <c r="E60" s="53" t="s">
         <v>110</v>
       </c>
-      <c r="F60" s="61"/>
+      <c r="F60" s="54"/>
       <c r="G60"/>
     </row>
-    <row r="61" spans="1:7" s="45" customFormat="1" ht="15" customHeight="1">
-      <c r="A61" s="29"/>
-      <c r="B61" s="43"/>
-      <c r="C61" s="44"/>
-      <c r="D61" s="44"/>
-      <c r="E61" s="60"/>
-      <c r="F61" s="61"/>
+    <row r="61" spans="1:7" s="45" customFormat="1" ht="15">
+      <c r="A61" s="29">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B61" s="48" t="s">
+        <v>111</v>
+      </c>
+      <c r="C61" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="D61" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="E61" s="53" t="s">
+        <v>112</v>
+      </c>
+      <c r="F61" s="54"/>
       <c r="G61"/>
     </row>
-    <row r="62" spans="1:7" s="45" customFormat="1">
-      <c r="A62" s="52"/>
-      <c r="B62" s="48"/>
+    <row r="62" spans="1:7" s="45" customFormat="1" ht="15" customHeight="1">
+      <c r="A62" s="29"/>
+      <c r="B62" s="43"/>
       <c r="C62" s="44"/>
-      <c r="D62" s="49"/>
-      <c r="E62" s="60"/>
-      <c r="F62" s="61"/>
+      <c r="D62" s="44"/>
+      <c r="E62" s="53"/>
+      <c r="F62" s="54"/>
       <c r="G62"/>
     </row>
-    <row r="63" spans="1:7">
-      <c r="A63" s="22"/>
-      <c r="B63" s="34"/>
-      <c r="C63" s="23"/>
-      <c r="D63" s="23"/>
-      <c r="E63" s="23"/>
-      <c r="F63" s="35"/>
+    <row r="63" spans="1:7" s="45" customFormat="1">
+      <c r="A63" s="52"/>
+      <c r="B63" s="48"/>
+      <c r="C63" s="44"/>
+      <c r="D63" s="49"/>
+      <c r="E63" s="53"/>
+      <c r="F63" s="54"/>
+      <c r="G63"/>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" s="22"/>
+      <c r="B64" s="34"/>
+      <c r="C64" s="23"/>
+      <c r="D64" s="23"/>
+      <c r="E64" s="23"/>
+      <c r="F64" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="38">
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="E54:F54"/>
+  <mergeCells count="39">
     <mergeCell ref="E61:F61"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="E60:F60"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E46:F46"/>
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:B20"/>
@@ -2719,10 +2727,37 @@
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="D25:D26"/>
     <mergeCell ref="E25:E26"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E63:F63"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="E60:F60"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations disablePrompts="1" count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D79" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D80" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
3.1.30 Adapt telegram generics.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestGeneratorKtTelegramStructure.xlsx
+++ b/meta/program/BlancoRestGeneratorKtTelegramStructure.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorKt/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A5192B9-7788-5C4C-9D86-3121AB18887E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06643E8-6B6E-BC43-9D7F-5E43710023A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2660" yWindow="3500" windowWidth="24320" windowHeight="17500" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="117">
   <si>
     <t>バリューオブジェクト定義書</t>
   </si>
@@ -692,6 +692,14 @@
     <rPh sb="10" eb="12">
       <t xml:space="preserve">カノウ </t>
     </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>generic</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>クラスの総称型を指定します。</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1301,6 +1309,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1321,21 +1344,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1728,7 +1736,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1772,7 +1780,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1797,10 +1805,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63:F63"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1973,23 +1981,23 @@
       <c r="F18"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="57" t="s">
+      <c r="A19" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="59"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="60"/>
+      <c r="C19" s="64"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="65"/>
       <c r="F19"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="57"/>
-      <c r="B20" s="58"/>
-      <c r="C20" s="59"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="60"/>
+      <c r="A20" s="62"/>
+      <c r="B20" s="63"/>
+      <c r="C20" s="64"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="65"/>
       <c r="F20"/>
     </row>
     <row r="21" spans="1:6">
@@ -2026,29 +2034,29 @@
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:6" ht="13.5" customHeight="1">
-      <c r="A25" s="57" t="s">
+      <c r="A25" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="57" t="s">
+      <c r="B25" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="61" t="s">
+      <c r="C25" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="D25" s="61" t="s">
+      <c r="D25" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="61" t="s">
+      <c r="E25" s="66" t="s">
         <v>7</v>
       </c>
       <c r="F25" s="26"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="57"/>
-      <c r="B26" s="57"/>
-      <c r="C26" s="61"/>
-      <c r="D26" s="61"/>
-      <c r="E26" s="61"/>
+      <c r="A26" s="62"/>
+      <c r="B26" s="62"/>
+      <c r="C26" s="66"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="66"/>
       <c r="F26" s="27"/>
     </row>
     <row r="27" spans="1:6">
@@ -2062,10 +2070,10 @@
         <v>24</v>
       </c>
       <c r="D27" s="19"/>
-      <c r="E27" s="55" t="s">
+      <c r="E27" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="F27" s="56"/>
+      <c r="F27" s="61"/>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="29">
@@ -2086,7 +2094,7 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="29">
-        <f t="shared" ref="A29:A62" si="0">A28+1</f>
+        <f t="shared" ref="A29:A63" si="0">A28+1</f>
         <v>3</v>
       </c>
       <c r="B29" s="30" t="s">
@@ -2154,8 +2162,8 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="29">
-        <f t="shared" si="0"/>
-        <v>7</v>
+        <f>A31+1</f>
+        <v>6</v>
       </c>
       <c r="B33" s="30" t="s">
         <v>25</v>
@@ -2171,106 +2179,103 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="29">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f>A32+1</f>
+        <v>7</v>
       </c>
       <c r="B34" s="30" t="s">
-        <v>44</v>
+        <v>115</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="D34" s="31"/>
       <c r="E34" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="F34" s="33"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="29">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B35" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="F34" s="33"/>
-    </row>
-    <row r="35" spans="1:7" s="45" customFormat="1" ht="45">
-      <c r="A35" s="29">
+      <c r="F35" s="33"/>
+    </row>
+    <row r="36" spans="1:7" s="45" customFormat="1" ht="45">
+      <c r="A36" s="29">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B35" s="43" t="s">
+      <c r="B36" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="44" t="s">
+      <c r="C36" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="D35" s="44" t="s">
+      <c r="D36" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="E35" s="62" t="s">
+      <c r="E36" s="55" t="s">
         <v>49</v>
       </c>
-      <c r="F35" s="63"/>
-      <c r="G35"/>
-    </row>
-    <row r="36" spans="1:7" s="45" customFormat="1" ht="15">
-      <c r="A36" s="29">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B36" s="43" t="s">
-        <v>56</v>
-      </c>
-      <c r="C36" s="44" t="s">
-        <v>57</v>
-      </c>
-      <c r="D36" s="44" t="s">
-        <v>58</v>
-      </c>
-      <c r="E36" s="53" t="s">
-        <v>59</v>
-      </c>
-      <c r="F36" s="54"/>
+      <c r="F36" s="56"/>
       <c r="G36"/>
     </row>
     <row r="37" spans="1:7" s="45" customFormat="1" ht="15">
       <c r="A37" s="29">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B37" s="43" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C37" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="D37" s="44"/>
+        <v>57</v>
+      </c>
+      <c r="D37" s="44" t="s">
+        <v>58</v>
+      </c>
       <c r="E37" s="53" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F37" s="54"/>
       <c r="G37"/>
     </row>
-    <row r="38" spans="1:7" s="45" customFormat="1" ht="45" customHeight="1">
+    <row r="38" spans="1:7" s="45" customFormat="1" ht="15">
       <c r="A38" s="29">
         <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B38" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" s="44"/>
+      <c r="E38" s="53" t="s">
+        <v>55</v>
+      </c>
+      <c r="F38" s="54"/>
+      <c r="G38"/>
+    </row>
+    <row r="39" spans="1:7" s="45" customFormat="1" ht="45" customHeight="1">
+      <c r="A39" s="29">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B38" s="43" t="s">
+      <c r="B39" s="43" t="s">
         <v>60</v>
-      </c>
-      <c r="C38" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="D38" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="E38" s="53" t="s">
-        <v>61</v>
-      </c>
-      <c r="F38" s="66"/>
-      <c r="G38"/>
-    </row>
-    <row r="39" spans="1:7" s="45" customFormat="1" ht="45">
-      <c r="A39" s="29">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B39" s="43" t="s">
-        <v>50</v>
       </c>
       <c r="C39" s="44" t="s">
         <v>47</v>
@@ -2279,95 +2284,96 @@
         <v>48</v>
       </c>
       <c r="E39" s="53" t="s">
-        <v>51</v>
-      </c>
-      <c r="F39" s="54"/>
+        <v>61</v>
+      </c>
+      <c r="F39" s="59"/>
       <c r="G39"/>
     </row>
     <row r="40" spans="1:7" s="45" customFormat="1" ht="45">
       <c r="A40" s="29">
         <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B40" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="D40" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="E40" s="53" t="s">
+        <v>51</v>
+      </c>
+      <c r="F40" s="54"/>
+      <c r="G40"/>
+    </row>
+    <row r="41" spans="1:7" s="45" customFormat="1" ht="45">
+      <c r="A41" s="29">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B40" s="46" t="s">
+      <c r="B41" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="C40" s="47" t="s">
+      <c r="C41" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="D40" s="47" t="s">
+      <c r="D41" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="E40" s="64" t="s">
+      <c r="E41" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="F40" s="65"/>
-      <c r="G40"/>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="29">
+      <c r="F41" s="58"/>
+      <c r="G41"/>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="29">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B41" s="51" t="s">
+      <c r="B42" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="C41" s="51" t="s">
+      <c r="C42" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="D41" s="51" t="s">
+      <c r="D42" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="E41" s="50" t="s">
+      <c r="E42" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="F41" s="42"/>
-    </row>
-    <row r="42" spans="1:7" ht="15">
-      <c r="A42" s="29">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B42" s="43" t="s">
-        <v>67</v>
-      </c>
-      <c r="C42" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="D42" s="44" t="s">
-        <v>68</v>
-      </c>
-      <c r="E42" s="53" t="s">
-        <v>69</v>
-      </c>
-      <c r="F42" s="54"/>
+      <c r="F42" s="42"/>
     </row>
     <row r="43" spans="1:7" ht="15">
       <c r="A43" s="29">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B43" s="43" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C43" s="44" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="D43" s="44" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="E43" s="53" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F43" s="54"/>
     </row>
     <row r="44" spans="1:7" ht="15">
       <c r="A44" s="29">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B44" s="43" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C44" s="44" t="s">
         <v>57</v>
@@ -2376,17 +2382,17 @@
         <v>58</v>
       </c>
       <c r="E44" s="53" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F44" s="54"/>
     </row>
-    <row r="45" spans="1:7" s="45" customFormat="1" ht="15">
+    <row r="45" spans="1:7" ht="15">
       <c r="A45" s="29">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B45" s="43" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C45" s="44" t="s">
         <v>57</v>
@@ -2395,45 +2401,46 @@
         <v>58</v>
       </c>
       <c r="E45" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="F45" s="54"/>
+    </row>
+    <row r="46" spans="1:7" s="45" customFormat="1" ht="15">
+      <c r="A46" s="29">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B46" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="C46" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="D46" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="E46" s="53" t="s">
         <v>75</v>
-      </c>
-      <c r="F45" s="54"/>
-      <c r="G45"/>
-    </row>
-    <row r="46" spans="1:7" s="45" customFormat="1">
-      <c r="A46" s="29">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B46" s="48" t="s">
-        <v>76</v>
-      </c>
-      <c r="C46" s="49" t="s">
-        <v>77</v>
-      </c>
-      <c r="D46" s="49" t="s">
-        <v>78</v>
-      </c>
-      <c r="E46" s="53" t="s">
-        <v>79</v>
       </c>
       <c r="F46" s="54"/>
       <c r="G46"/>
     </row>
-    <row r="47" spans="1:7" s="45" customFormat="1" ht="15">
+    <row r="47" spans="1:7" s="45" customFormat="1">
       <c r="A47" s="29">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B47" s="48" t="s">
-        <v>80</v>
-      </c>
-      <c r="C47" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="D47" s="49"/>
+        <v>76</v>
+      </c>
+      <c r="C47" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="D47" s="49" t="s">
+        <v>78</v>
+      </c>
       <c r="E47" s="53" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F47" s="54"/>
       <c r="G47"/>
@@ -2441,17 +2448,17 @@
     <row r="48" spans="1:7" s="45" customFormat="1" ht="15">
       <c r="A48" s="29">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B48" s="48" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C48" s="44" t="s">
         <v>34</v>
       </c>
       <c r="D48" s="49"/>
       <c r="E48" s="53" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F48" s="54"/>
       <c r="G48"/>
@@ -2459,37 +2466,35 @@
     <row r="49" spans="1:7" s="45" customFormat="1" ht="15">
       <c r="A49" s="29">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B49" s="48" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C49" s="44" t="s">
         <v>34</v>
       </c>
       <c r="D49" s="49"/>
       <c r="E49" s="53" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F49" s="54"/>
       <c r="G49"/>
     </row>
-    <row r="50" spans="1:7" s="45" customFormat="1" ht="15" customHeight="1">
+    <row r="50" spans="1:7" s="45" customFormat="1" ht="15">
       <c r="A50" s="29">
         <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B50" s="43" t="s">
-        <v>86</v>
+        <v>23</v>
+      </c>
+      <c r="B50" s="48" t="s">
+        <v>84</v>
       </c>
       <c r="C50" s="44" t="s">
-        <v>57</v>
-      </c>
-      <c r="D50" s="44" t="b">
-        <v>0</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="D50" s="49"/>
       <c r="E50" s="53" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F50" s="54"/>
       <c r="G50"/>
@@ -2497,17 +2502,19 @@
     <row r="51" spans="1:7" s="45" customFormat="1" ht="15" customHeight="1">
       <c r="A51" s="29">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B51" s="43" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C51" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="D51" s="44"/>
+        <v>57</v>
+      </c>
+      <c r="D51" s="44" t="b">
+        <v>0</v>
+      </c>
       <c r="E51" s="53" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F51" s="54"/>
       <c r="G51"/>
@@ -2515,17 +2522,17 @@
     <row r="52" spans="1:7" s="45" customFormat="1" ht="15" customHeight="1">
       <c r="A52" s="29">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B52" s="43" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C52" s="44" t="s">
         <v>34</v>
       </c>
       <c r="D52" s="44"/>
       <c r="E52" s="53" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F52" s="54"/>
       <c r="G52"/>
@@ -2533,17 +2540,17 @@
     <row r="53" spans="1:7" s="45" customFormat="1" ht="15" customHeight="1">
       <c r="A53" s="29">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B53" s="43" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C53" s="44" t="s">
         <v>34</v>
       </c>
       <c r="D53" s="44"/>
       <c r="E53" s="53" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F53" s="54"/>
       <c r="G53"/>
@@ -2551,19 +2558,17 @@
     <row r="54" spans="1:7" s="45" customFormat="1" ht="15" customHeight="1">
       <c r="A54" s="29">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B54" s="43" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C54" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="D54" s="44" t="s">
-        <v>95</v>
-      </c>
+      <c r="D54" s="44"/>
       <c r="E54" s="53" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F54" s="54"/>
       <c r="G54"/>
@@ -2571,75 +2576,75 @@
     <row r="55" spans="1:7" s="45" customFormat="1" ht="15" customHeight="1">
       <c r="A55" s="29">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B55" s="43" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C55" s="44" t="s">
-        <v>57</v>
-      </c>
-      <c r="D55" s="44" t="b">
-        <v>0</v>
+        <v>34</v>
+      </c>
+      <c r="D55" s="44" t="s">
+        <v>95</v>
       </c>
       <c r="E55" s="53" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F55" s="54"/>
       <c r="G55"/>
     </row>
-    <row r="56" spans="1:7" s="45" customFormat="1" ht="15">
+    <row r="56" spans="1:7" s="45" customFormat="1" ht="15" customHeight="1">
       <c r="A56" s="29">
         <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="B56" s="48" t="s">
-        <v>99</v>
+        <v>29</v>
+      </c>
+      <c r="B56" s="43" t="s">
+        <v>97</v>
       </c>
       <c r="C56" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="D56" s="49"/>
+        <v>57</v>
+      </c>
+      <c r="D56" s="44" t="b">
+        <v>0</v>
+      </c>
       <c r="E56" s="53" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F56" s="54"/>
       <c r="G56"/>
     </row>
-    <row r="57" spans="1:7" s="45" customFormat="1" ht="45">
+    <row r="57" spans="1:7" s="45" customFormat="1" ht="15">
       <c r="A57" s="29">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B57" s="48" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C57" s="44" t="s">
-        <v>102</v>
+        <v>34</v>
       </c>
       <c r="D57" s="49"/>
       <c r="E57" s="53" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F57" s="54"/>
       <c r="G57"/>
     </row>
-    <row r="58" spans="1:7" s="45" customFormat="1" ht="15">
+    <row r="58" spans="1:7" s="45" customFormat="1" ht="45">
       <c r="A58" s="29">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B58" s="48" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C58" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="D58" s="49" t="s">
-        <v>105</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="D58" s="49"/>
       <c r="E58" s="53" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F58" s="54"/>
       <c r="G58"/>
@@ -2647,19 +2652,19 @@
     <row r="59" spans="1:7" s="45" customFormat="1" ht="15">
       <c r="A59" s="29">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B59" s="48" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C59" s="44" t="s">
-        <v>57</v>
-      </c>
-      <c r="D59" s="49" t="b">
-        <v>0</v>
+        <v>34</v>
+      </c>
+      <c r="D59" s="49" t="s">
+        <v>105</v>
       </c>
       <c r="E59" s="53" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F59" s="54"/>
       <c r="G59"/>
@@ -2667,10 +2672,10 @@
     <row r="60" spans="1:7" s="45" customFormat="1" ht="15">
       <c r="A60" s="29">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B60" s="48" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C60" s="44" t="s">
         <v>57</v>
@@ -2679,7 +2684,7 @@
         <v>0</v>
       </c>
       <c r="E60" s="53" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F60" s="54"/>
       <c r="G60"/>
@@ -2687,19 +2692,19 @@
     <row r="61" spans="1:7" s="45" customFormat="1" ht="15">
       <c r="A61" s="29">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B61" s="48" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C61" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="D61" s="49" t="s">
-        <v>105</v>
+        <v>57</v>
+      </c>
+      <c r="D61" s="49" t="b">
+        <v>0</v>
       </c>
       <c r="E61" s="53" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F61" s="54"/>
       <c r="G61"/>
@@ -2707,76 +2712,71 @@
     <row r="62" spans="1:7" s="45" customFormat="1" ht="15">
       <c r="A62" s="29">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B62" s="48" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C62" s="44" t="s">
-        <v>57</v>
-      </c>
-      <c r="D62" s="49" t="b">
-        <v>0</v>
+        <v>34</v>
+      </c>
+      <c r="D62" s="49" t="s">
+        <v>105</v>
       </c>
       <c r="E62" s="53" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F62" s="54"/>
       <c r="G62"/>
     </row>
-    <row r="63" spans="1:7" s="45" customFormat="1" ht="15" customHeight="1">
-      <c r="A63" s="29"/>
-      <c r="B63" s="43"/>
-      <c r="C63" s="44"/>
-      <c r="D63" s="44"/>
-      <c r="E63" s="53"/>
+    <row r="63" spans="1:7" s="45" customFormat="1" ht="15">
+      <c r="A63" s="29">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B63" s="48" t="s">
+        <v>113</v>
+      </c>
+      <c r="C63" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="D63" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="E63" s="53" t="s">
+        <v>114</v>
+      </c>
       <c r="F63" s="54"/>
       <c r="G63"/>
     </row>
-    <row r="64" spans="1:7" s="45" customFormat="1">
-      <c r="A64" s="52"/>
-      <c r="B64" s="48"/>
+    <row r="64" spans="1:7" s="45" customFormat="1" ht="15" customHeight="1">
+      <c r="A64" s="29"/>
+      <c r="B64" s="43"/>
       <c r="C64" s="44"/>
-      <c r="D64" s="49"/>
+      <c r="D64" s="44"/>
       <c r="E64" s="53"/>
       <c r="F64" s="54"/>
       <c r="G64"/>
     </row>
-    <row r="65" spans="1:6">
-      <c r="A65" s="22"/>
-      <c r="B65" s="34"/>
-      <c r="C65" s="23"/>
-      <c r="D65" s="23"/>
-      <c r="E65" s="23"/>
-      <c r="F65" s="35"/>
+    <row r="65" spans="1:7" s="45" customFormat="1">
+      <c r="A65" s="52"/>
+      <c r="B65" s="48"/>
+      <c r="C65" s="44"/>
+      <c r="D65" s="49"/>
+      <c r="E65" s="53"/>
+      <c r="F65" s="54"/>
+      <c r="G65"/>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" s="22"/>
+      <c r="B66" s="34"/>
+      <c r="C66" s="23"/>
+      <c r="D66" s="23"/>
+      <c r="E66" s="23"/>
+      <c r="F66" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E64:F64"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="E63:F63"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="E60:F60"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E61:F61"/>
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:B20"/>
@@ -2788,14 +2788,39 @@
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="D25:D26"/>
     <mergeCell ref="E25:E26"/>
-    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E39:F39"/>
     <mergeCell ref="E43:F43"/>
     <mergeCell ref="E44:F44"/>
     <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E65:F65"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="E64:F64"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="E61:F61"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="E63:F63"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E49:F49"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations disablePrompts="1" count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D81" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D82" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>